<commit_message>
canvi de llistes a diccionari
</commit_message>
<xml_diff>
--- a/Hores.xlsx
+++ b/Hores.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>Agost</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>Setembre</t>
+  </si>
+  <si>
+    <t>3h</t>
   </si>
 </sst>
 </file>
@@ -362,7 +365,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -419,16 +422,25 @@
       <c r="A7">
         <v>21</v>
       </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
         <v>24</v>
       </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
         <v>25</v>
       </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10">
@@ -447,6 +459,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>